<commit_message>
mods to behavioral health spreadsheet for meeting with CRC
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Behavioral_Health_Evalutation_Reporting_Service_SSP_v.1.0.0/artifacts/service_model/information_model/BehavioralHealthRecord_IEPD/documentation/BehaviorHealthReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Behavioral_Health_Evalutation_Reporting_Service_SSP_v.1.0.0/artifacts/service_model/information_model/BehavioralHealthRecord_IEPD/documentation/BehaviorHealthReportMapping.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Behavioral Health Reporting" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -219,9 +219,6 @@
     <t>code or description of the type of mental health disorder (CT: Master Problems List)</t>
   </si>
   <si>
-    <t>Behavior Health Report Mapping</t>
-  </si>
-  <si>
     <t>/bhr-doc:BehaviorHealthReport/nc:DocumentCreationDate/nc:DateTime</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>/bhr-doc:BehaviorHealthReport/brh-ext:BehaviorHealthAssessment/bhr-ext:SeriousMentalHealthTypeCategoryText</t>
+  </si>
+  <si>
+    <t>Behavioral Health Report Mapping</t>
   </si>
 </sst>
 </file>
@@ -1194,14 +1194,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="666">
@@ -2207,8 +2207,8 @@
   <dimension ref="A1:H354"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2225,10 +2225,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="28"/>
+      <c r="A1" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="29"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -2279,7 +2279,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>9</v>
@@ -2300,7 +2300,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -2332,7 +2332,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -2353,7 +2353,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -2385,7 +2385,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>15</v>
@@ -2406,7 +2406,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -2423,7 +2423,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
@@ -2443,7 +2443,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -2461,7 +2461,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="17" t="s">
@@ -2479,7 +2479,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>15</v>
@@ -2501,7 +2501,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>15</v>
@@ -2523,7 +2523,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>15</v>
@@ -2545,7 +2545,7 @@
         <v>28</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>15</v>
@@ -2575,7 +2575,7 @@
         <v>48</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>15</v>
@@ -2596,7 +2596,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>15</v>
@@ -2615,7 +2615,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
@@ -2642,8 +2642,8 @@
       <c r="C24" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>83</v>
+      <c r="D24" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>15</v>
@@ -2660,7 +2660,7 @@
         <v>49</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="19" t="s">
@@ -2678,7 +2678,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="19" t="s">
@@ -2696,7 +2696,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="19" t="s">
@@ -2706,15 +2706,15 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
+      <c r="A28" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
@@ -2728,7 +2728,7 @@
         <v>55</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
@@ -2748,7 +2748,7 @@
         <v>57</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
@@ -2768,7 +2768,7 @@
         <v>59</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="26"/>
@@ -2788,7 +2788,7 @@
         <v>61</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E32" s="27"/>
       <c r="F32" s="26"/>
@@ -2808,7 +2808,7 @@
         <v>63</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="26"/>
@@ -2828,7 +2828,7 @@
         <v>65</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>

</xml_diff>